<commit_message>
Se agregan validaciones para subir planilla validadora, queda validar mas columnas
</commit_message>
<xml_diff>
--- a/macro_vtf/analyst/static/plantillas/plantilla_validadora.xlsx
+++ b/macro_vtf/analyst/static/plantillas/plantilla_validadora.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snavarro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\snavarro\dev\python\django_macro\macro_vtf\analyst\static\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BEBB8E-B24D-4E14-B27F-A443B2595914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C68FC4-4FC9-4366-8701-3EEF3B491861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>MES</t>
   </si>
@@ -36,144 +36,18 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>APELLIDO PATERNO</t>
-  </si>
-  <si>
-    <t>APELLIDO MATERNO</t>
-  </si>
-  <si>
-    <t>FECHA DE NACIMIENTO</t>
-  </si>
-  <si>
     <t>CARGO</t>
   </si>
   <si>
     <t>GRUPO</t>
   </si>
   <si>
-    <t>NIVEL DE 
-ATENCIÓN</t>
-  </si>
-  <si>
-    <t>FECHA DE INGRESO AL SISTEMA ESCOLAR</t>
-  </si>
-  <si>
-    <t>AÑOS DE SERVICIO CON EL EMPLEADOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FECHA ESTABLECIDA EN 
-CONTRATO DE TRABAJO </t>
-  </si>
-  <si>
-    <t>JORNADA/HORAS</t>
-  </si>
-  <si>
-    <t>PLAZO DEL 
-CONTRATO</t>
-  </si>
-  <si>
-    <t>TIPO DE CONTRATO</t>
-  </si>
-  <si>
-    <t>NIVEL EDUCACIONAL</t>
-  </si>
-  <si>
-    <t>TÍTULO</t>
-  </si>
-  <si>
-    <t>INSTITUCIÓN ACADÉMICA</t>
-  </si>
-  <si>
-    <t>DÍAS DE LICENCIA MÉDICA</t>
-  </si>
-  <si>
-    <t>DÍAS SIN GOCE DE SUELDO</t>
-  </si>
-  <si>
-    <t>TOTAL DÍAS TRABAJADOS</t>
-  </si>
-  <si>
-    <t>TOTAL DÍAS PAGADOS</t>
-  </si>
-  <si>
-    <t>(Remuneraciones )INCLUYE BONOS Y ASIGNACIONES PACTADAS</t>
-  </si>
-  <si>
-    <t>MOVILIZACIÓN MÁS COLACIÓN</t>
-  </si>
-  <si>
-    <t>MES Y AÑO DE INICIO DEL PAGO</t>
-  </si>
-  <si>
-    <t>ASIGNACIÓN MENSUAL SOLICITADA (CD)</t>
-  </si>
-  <si>
-    <t>SUELDO BASE</t>
-  </si>
-  <si>
-    <t>HORAS EXTRAS</t>
-  </si>
-  <si>
-    <t>ANTIGÜEDAD /BIENIOS</t>
-  </si>
-  <si>
     <t>INCENTIVO</t>
   </si>
   <si>
-    <t xml:space="preserve">ASIGNACIÓN DE RESPONSABILIDAD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELIQUIDACIONES </t>
-  </si>
-  <si>
-    <t>INCREMENTOS JUNJI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGUINALDO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASIGNACIÓN ZONA EXTREMA </t>
-  </si>
-  <si>
     <t>BONO</t>
   </si>
   <si>
-    <t xml:space="preserve">OTROS AJUSTES </t>
-  </si>
-  <si>
-    <t>ESPECÍFIQUE</t>
-  </si>
-  <si>
-    <t>BONO VACACIONES FISCAL</t>
-  </si>
-  <si>
-    <t>BONO TÉRMINO DE CONFLICTO FISCAL</t>
-  </si>
-  <si>
-    <t>BONO ESCOLAR</t>
-  </si>
-  <si>
-    <t>MOVILIZACIÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLACIÓN </t>
-  </si>
-  <si>
-    <t>ASIGNACIONES FAMILIARES</t>
-  </si>
-  <si>
-    <t>ASIGNACIÓN LEY 20.905</t>
-  </si>
-  <si>
-    <t>OTROS AJUSTES</t>
-  </si>
-  <si>
-    <t>ASIGNACIÓN CARRERA DOCENTE PAGADA</t>
-  </si>
-  <si>
-    <t>SUELDO BRUTO O TOTAL HABERES</t>
-  </si>
-  <si>
     <t>OBSERVACIONES</t>
   </si>
   <si>
@@ -187,6 +61,138 @@
   </si>
   <si>
     <t>FUNCION</t>
+  </si>
+  <si>
+    <t>APELLIDO_PATERNO</t>
+  </si>
+  <si>
+    <t>APELLIDO_MATERNO</t>
+  </si>
+  <si>
+    <t>FECHA_NACIMIENTO</t>
+  </si>
+  <si>
+    <t>NIVEL_ATENCION</t>
+  </si>
+  <si>
+    <t>FECHA_INGRESO_SISTEMA_ESCOLAR</t>
+  </si>
+  <si>
+    <t>ANIOS_SERVICIO_CON_EMPLEADOR</t>
+  </si>
+  <si>
+    <t>FECHA_ESTABLECIDA_CONTRATO</t>
+  </si>
+  <si>
+    <t>JORNADA_HORAS</t>
+  </si>
+  <si>
+    <t>PLAZO_CONTRATO</t>
+  </si>
+  <si>
+    <t>TIPO_CONTRATO</t>
+  </si>
+  <si>
+    <t>NIVEL_EDUCACIONAL</t>
+  </si>
+  <si>
+    <t>TITULO</t>
+  </si>
+  <si>
+    <t>INSTITUCION_ACADEMICA</t>
+  </si>
+  <si>
+    <t>DIAS_LICENCIA_MEDICA</t>
+  </si>
+  <si>
+    <t>DIAS_SIN_GOCE_SUELDO</t>
+  </si>
+  <si>
+    <t>TOTAL_DIAS_TRABAJADOS</t>
+  </si>
+  <si>
+    <t>TOTAL_DIAS_PAGADOS</t>
+  </si>
+  <si>
+    <t>REMUNERACIONES_INCLUYE_BONOS_Y_ASIGNACIONES_PACTADAS</t>
+  </si>
+  <si>
+    <t>MOVILIZACION_MAS_COLACION</t>
+  </si>
+  <si>
+    <t>MES_Y_ANIO_INICIO_PAGO</t>
+  </si>
+  <si>
+    <t>ASIGNACION_MENSUAL_SOLICITADA_DE_CD</t>
+  </si>
+  <si>
+    <t>SUELDO_BASE</t>
+  </si>
+  <si>
+    <t>HORAS_EXTRAS</t>
+  </si>
+  <si>
+    <t>ANTIGUEDAD_BIENIOS</t>
+  </si>
+  <si>
+    <t>INCREMENTOS_JUNJI</t>
+  </si>
+  <si>
+    <t>ESPECIFIQUE</t>
+  </si>
+  <si>
+    <t>BONO_VACACIONES_FISCAL</t>
+  </si>
+  <si>
+    <t>BONO_TERMINO_CONFLICTO_FISCAL</t>
+  </si>
+  <si>
+    <t>BONO_ESCOLAR</t>
+  </si>
+  <si>
+    <t>MOVILIZACION</t>
+  </si>
+  <si>
+    <t>ASIGNACIONES_FAMILIARES</t>
+  </si>
+  <si>
+    <t>ASIGNACION_LEY_20905</t>
+  </si>
+  <si>
+    <t>OTROS_AJUSTES</t>
+  </si>
+  <si>
+    <t>ASIGNACION_CARRERA_DOCENTE_PAGADA</t>
+  </si>
+  <si>
+    <t>SUELDO_BRUTO_O_TOTAL_HABERES</t>
+  </si>
+  <si>
+    <t>ASIGNACION_RESPONSABILIDAD</t>
+  </si>
+  <si>
+    <t>RELIQUIDACIONES</t>
+  </si>
+  <si>
+    <t>AGUINALDO</t>
+  </si>
+  <si>
+    <t>ASIGNACION_ZONA_EXTREMA</t>
+  </si>
+  <si>
+    <t>AGUINALDO_2</t>
+  </si>
+  <si>
+    <t>BONO_2</t>
+  </si>
+  <si>
+    <t>ESPECIFIQUE_2</t>
+  </si>
+  <si>
+    <t>COLACION</t>
+  </si>
+  <si>
+    <t>OTROS_AJUSTES_2</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AU1" sqref="AU1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -592,13 +600,13 @@
   <sheetData>
     <row r="1" spans="1:56" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -610,109 +618,109 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="AO1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>37</v>
@@ -724,7 +732,7 @@
         <v>39</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>40</v>
@@ -733,31 +741,31 @@
         <v>41</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="AW1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AZ1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BC1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="BD1" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>